<commit_message>
Added more data to test_result
</commit_message>
<xml_diff>
--- a/data/test_result.xlsx
+++ b/data/test_result.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Research\NLP4Kaomoji\ASCII-Art-Identifier\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6160023D-67B8-40F2-8EF3-01C8F320A957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="27950" windowHeight="12280"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,8 +26,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -29,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="68">
   <si>
     <t>id</t>
   </si>
@@ -190,56 +194,56 @@
     <t>kaomoji_e38e8259</t>
   </si>
   <si>
-    <t>kaomoji_ecf28394</t>
-  </si>
-  <si>
     <t>multiline</t>
   </si>
   <si>
-    <t>kaomoji_ee7313e4</t>
-  </si>
-  <si>
-    <t>kaomoji_eff0e3d6</t>
-  </si>
-  <si>
-    <t>kaomoji_f20dfcf3</t>
-  </si>
-  <si>
-    <t>kaomoji_f50525ec</t>
-  </si>
-  <si>
-    <t>kaomoji_f5935c1c</t>
-  </si>
-  <si>
-    <t>kaomoji_f6936e0a</t>
-  </si>
-  <si>
-    <t>kaomoji_f899963a</t>
-  </si>
-  <si>
-    <t>kaomoji_f98cfb73</t>
-  </si>
-  <si>
-    <t>kaomoji_fa8eb34d</t>
-  </si>
-  <si>
-    <t>kaomoji_fe202a57</t>
-  </si>
-  <si>
-    <t>kaomoji_fa8qs34d</t>
+    <t>multiline_ecf28394</t>
+  </si>
+  <si>
+    <t>multiline_ee7313e4</t>
+  </si>
+  <si>
+    <t>multiline_eff0e3d6</t>
+  </si>
+  <si>
+    <t>multiline_f20dfcf3</t>
+  </si>
+  <si>
+    <t>multiline_f50525ec</t>
+  </si>
+  <si>
+    <t>multiline_f5935c1c</t>
+  </si>
+  <si>
+    <t>multiline_f6936e0a</t>
+  </si>
+  <si>
+    <t>multiline_f899963a</t>
+  </si>
+  <si>
+    <t>multiline_f98cfb73</t>
+  </si>
+  <si>
+    <t>multiline_fa8eb34d</t>
+  </si>
+  <si>
+    <t>multiline_fe202a57</t>
+  </si>
+  <si>
+    <t>multiline_fa8qs34d</t>
+  </si>
+  <si>
+    <t>multiline_fa8qs45d</t>
+  </si>
+  <si>
+    <t>multiline_fa8rs16w</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="20">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -248,345 +252,36 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="9"/>
       <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -594,251 +289,9 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -846,65 +299,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
-    <cellStyle name="货币" xfId="2" builtinId="4"/>
-    <cellStyle name="百分比" xfId="3" builtinId="5"/>
-    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
-    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
-    <cellStyle name="超链接" xfId="6" builtinId="8"/>
-    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
-    <cellStyle name="注释" xfId="8" builtinId="10"/>
-    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
-    <cellStyle name="标题" xfId="10" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
-    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="输入" xfId="16" builtinId="20"/>
-    <cellStyle name="输出" xfId="17" builtinId="21"/>
-    <cellStyle name="计算" xfId="18" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
-    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
-    <cellStyle name="汇总" xfId="21" builtinId="25"/>
-    <cellStyle name="好" xfId="22" builtinId="26"/>
-    <cellStyle name="差" xfId="23" builtinId="27"/>
-    <cellStyle name="适中" xfId="24" builtinId="28"/>
-    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
-    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
-    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
-    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
-    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1154,38 +563,37 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:J154"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J160"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="H138" sqref="H138"/>
+      <pane ySplit="1" topLeftCell="A138" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I160" sqref="I160"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5454545454545" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.81818181818182" style="1"/>
-    <col min="3" max="3" width="29.8181818181818" customWidth="1"/>
+    <col min="1" max="1" width="22.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.81640625"/>
+    <col min="3" max="3" width="29.81640625" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="28.6363636363636" customWidth="1"/>
-    <col min="6" max="6" width="27.5454545454545" customWidth="1"/>
-    <col min="8" max="8" width="28.6363636363636" customWidth="1"/>
-    <col min="9" max="9" width="27.5454545454545" customWidth="1"/>
-    <col min="10" max="10" width="17.3636363636364" customWidth="1"/>
+    <col min="5" max="5" width="28.6328125" customWidth="1"/>
+    <col min="6" max="6" width="27.54296875" customWidth="1"/>
+    <col min="8" max="8" width="28.6328125" customWidth="1"/>
+    <col min="9" max="9" width="27.54296875" customWidth="1"/>
+    <col min="10" max="10" width="17.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -1213,11 +621,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>11</v>
       </c>
       <c r="C2">
@@ -1245,11 +653,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>11</v>
       </c>
       <c r="C3">
@@ -1277,11 +685,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>11</v>
       </c>
       <c r="C4">
@@ -1309,11 +717,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>11</v>
       </c>
       <c r="C5">
@@ -1341,11 +749,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>11</v>
       </c>
       <c r="C6">
@@ -1373,11 +781,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>11</v>
       </c>
       <c r="C7">
@@ -1405,11 +813,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>11</v>
       </c>
       <c r="C8">
@@ -1437,11 +845,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>11</v>
       </c>
       <c r="C9">
@@ -1469,11 +877,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>11</v>
       </c>
       <c r="C10">
@@ -1501,11 +909,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>11</v>
       </c>
       <c r="C11">
@@ -1533,11 +941,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>11</v>
       </c>
       <c r="C12">
@@ -1565,11 +973,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>11</v>
       </c>
       <c r="C13">
@@ -1597,11 +1005,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>11</v>
       </c>
       <c r="C14">
@@ -1629,11 +1037,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>11</v>
       </c>
       <c r="C15">
@@ -1661,11 +1069,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>11</v>
       </c>
       <c r="C16">
@@ -1693,11 +1101,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>11</v>
       </c>
       <c r="C17">
@@ -1725,11 +1133,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>11</v>
       </c>
       <c r="C18">
@@ -1739,10 +1147,10 @@
         <v>0</v>
       </c>
       <c r="E18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18">
         <v>0</v>
@@ -1757,11 +1165,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>11</v>
       </c>
       <c r="C19">
@@ -1771,10 +1179,10 @@
         <v>0</v>
       </c>
       <c r="E19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19">
         <v>0</v>
@@ -1789,11 +1197,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>11</v>
       </c>
       <c r="C20">
@@ -1803,10 +1211,10 @@
         <v>0</v>
       </c>
       <c r="E20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -1821,11 +1229,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>11</v>
       </c>
       <c r="C21">
@@ -1835,7 +1243,7 @@
         <v>0</v>
       </c>
       <c r="E21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F21">
         <v>0</v>
@@ -1853,11 +1261,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" t="s">
         <v>11</v>
       </c>
       <c r="C22">
@@ -1885,18 +1293,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
-      <c r="A23" s="1" t="s">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" t="s">
         <v>11</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23">
         <v>1</v>
@@ -1917,11 +1325,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
-      <c r="A24" s="1" t="s">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" t="s">
         <v>11</v>
       </c>
       <c r="C24">
@@ -1949,11 +1357,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
-      <c r="A25" s="1" t="s">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" t="s">
         <v>11</v>
       </c>
       <c r="C25">
@@ -1981,11 +1389,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
-      <c r="A26" s="1" t="s">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" t="s">
         <v>11</v>
       </c>
       <c r="C26">
@@ -2013,11 +1421,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
-      <c r="A27" s="1" t="s">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" t="s">
         <v>11</v>
       </c>
       <c r="C27">
@@ -2045,18 +1453,18 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
-      <c r="A28" s="1" t="s">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" t="s">
         <v>11</v>
       </c>
       <c r="C28">
         <v>1</v>
       </c>
       <c r="D28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28">
         <v>1</v>
@@ -2077,11 +1485,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
-      <c r="A29" s="1" t="s">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>23</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" t="s">
         <v>11</v>
       </c>
       <c r="C29">
@@ -2109,11 +1517,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
-      <c r="A30" s="1" t="s">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" t="s">
         <v>11</v>
       </c>
       <c r="C30">
@@ -2141,11 +1549,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
-      <c r="A31" s="1" t="s">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>23</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" t="s">
         <v>11</v>
       </c>
       <c r="C31">
@@ -2173,11 +1581,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
-      <c r="A32" s="1" t="s">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>24</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" t="s">
         <v>11</v>
       </c>
       <c r="C32">
@@ -2205,11 +1613,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
-      <c r="A33" s="1" t="s">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>24</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" t="s">
         <v>11</v>
       </c>
       <c r="C33">
@@ -2237,11 +1645,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
-      <c r="A34" s="1" t="s">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>24</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" t="s">
         <v>11</v>
       </c>
       <c r="C34">
@@ -2269,11 +1677,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
-      <c r="A35" s="1" t="s">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>25</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" t="s">
         <v>11</v>
       </c>
       <c r="C35">
@@ -2301,11 +1709,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
-      <c r="A36" s="1" t="s">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>25</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" t="s">
         <v>11</v>
       </c>
       <c r="C36">
@@ -2333,11 +1741,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
-      <c r="A37" s="1" t="s">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>25</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" t="s">
         <v>11</v>
       </c>
       <c r="C37">
@@ -2365,11 +1773,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
-      <c r="A38" s="1" t="s">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>26</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" t="s">
         <v>11</v>
       </c>
       <c r="C38">
@@ -2397,11 +1805,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
-      <c r="A39" s="1" t="s">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>26</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" t="s">
         <v>11</v>
       </c>
       <c r="C39">
@@ -2429,11 +1837,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
-      <c r="A40" s="1" t="s">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>26</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" t="s">
         <v>11</v>
       </c>
       <c r="C40">
@@ -2461,11 +1869,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
-      <c r="A41" s="1" t="s">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>27</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" t="s">
         <v>11</v>
       </c>
       <c r="C41">
@@ -2493,11 +1901,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
-      <c r="A42" s="1" t="s">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>27</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" t="s">
         <v>11</v>
       </c>
       <c r="C42">
@@ -2525,11 +1933,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
-      <c r="A43" s="1" t="s">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>27</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" t="s">
         <v>11</v>
       </c>
       <c r="C43">
@@ -2557,11 +1965,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
-      <c r="A44" s="1" t="s">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>28</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" t="s">
         <v>11</v>
       </c>
       <c r="C44">
@@ -2589,11 +1997,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
-      <c r="A45" s="1" t="s">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>28</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" t="s">
         <v>11</v>
       </c>
       <c r="C45">
@@ -2621,11 +2029,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
-      <c r="A46" s="1" t="s">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>28</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" t="s">
         <v>11</v>
       </c>
       <c r="C46">
@@ -2653,11 +2061,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
-      <c r="A47" s="1" t="s">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>29</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" t="s">
         <v>11</v>
       </c>
       <c r="C47">
@@ -2685,18 +2093,18 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
-      <c r="A48" s="1" t="s">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>29</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" t="s">
         <v>11</v>
       </c>
       <c r="C48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E48">
         <v>1</v>
@@ -2717,11 +2125,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
-      <c r="A49" s="1" t="s">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>29</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B49" t="s">
         <v>11</v>
       </c>
       <c r="C49">
@@ -2749,11 +2157,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
-      <c r="A50" s="1" t="s">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>30</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B50" t="s">
         <v>11</v>
       </c>
       <c r="C50">
@@ -2781,11 +2189,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
-      <c r="A51" s="1" t="s">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>30</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B51" t="s">
         <v>11</v>
       </c>
       <c r="C51">
@@ -2813,11 +2221,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" customFormat="1" spans="1:10">
-      <c r="A52" s="1" t="s">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>30</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B52" t="s">
         <v>11</v>
       </c>
       <c r="C52">
@@ -2845,18 +2253,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="53" customFormat="1" spans="1:10">
-      <c r="A53" s="1" t="s">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>31</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B53" t="s">
         <v>11</v>
       </c>
       <c r="C53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E53">
         <v>1</v>
@@ -2877,18 +2285,18 @@
         <v>12</v>
       </c>
     </row>
-    <row r="54" customFormat="1" spans="1:10">
-      <c r="A54" s="1" t="s">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>31</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B54" t="s">
         <v>11</v>
       </c>
       <c r="C54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E54">
         <v>1</v>
@@ -2909,18 +2317,18 @@
         <v>13</v>
       </c>
     </row>
-    <row r="55" customFormat="1" spans="1:10">
-      <c r="A55" s="1" t="s">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>31</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B55" t="s">
         <v>11</v>
       </c>
       <c r="C55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E55">
         <v>1</v>
@@ -2941,11 +2349,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="56" customFormat="1" spans="1:10">
-      <c r="A56" s="1" t="s">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>32</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B56" t="s">
         <v>11</v>
       </c>
       <c r="C56">
@@ -2973,11 +2381,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="57" customFormat="1" spans="1:10">
-      <c r="A57" s="1" t="s">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>32</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B57" t="s">
         <v>11</v>
       </c>
       <c r="C57">
@@ -3005,11 +2413,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="58" customFormat="1" spans="1:10">
-      <c r="A58" s="1" t="s">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>32</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B58" t="s">
         <v>11</v>
       </c>
       <c r="C58">
@@ -3037,11 +2445,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="59" customFormat="1" spans="1:10">
-      <c r="A59" s="1" t="s">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>33</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B59" t="s">
         <v>11</v>
       </c>
       <c r="C59">
@@ -3069,11 +2477,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="60" customFormat="1" spans="1:10">
-      <c r="A60" s="1" t="s">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>33</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B60" t="s">
         <v>11</v>
       </c>
       <c r="C60">
@@ -3101,11 +2509,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="61" customFormat="1" spans="1:10">
-      <c r="A61" s="1" t="s">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>33</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B61" t="s">
         <v>11</v>
       </c>
       <c r="C61">
@@ -3133,11 +2541,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="62" customFormat="1" spans="1:10">
-      <c r="A62" s="1" t="s">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>34</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B62" t="s">
         <v>11</v>
       </c>
       <c r="C62">
@@ -3165,11 +2573,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="63" customFormat="1" spans="1:10">
-      <c r="A63" s="1" t="s">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>34</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B63" t="s">
         <v>11</v>
       </c>
       <c r="C63">
@@ -3197,11 +2605,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="64" customFormat="1" spans="1:10">
-      <c r="A64" s="1" t="s">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>34</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B64" t="s">
         <v>11</v>
       </c>
       <c r="C64">
@@ -3229,11 +2637,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="65" customFormat="1" spans="1:10">
-      <c r="A65" s="1" t="s">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>35</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B65" t="s">
         <v>11</v>
       </c>
       <c r="C65">
@@ -3261,11 +2669,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="66" customFormat="1" spans="1:10">
-      <c r="A66" s="1" t="s">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>35</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B66" t="s">
         <v>11</v>
       </c>
       <c r="C66">
@@ -3293,11 +2701,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="67" customFormat="1" spans="1:10">
-      <c r="A67" s="1" t="s">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>35</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B67" t="s">
         <v>11</v>
       </c>
       <c r="C67">
@@ -3325,11 +2733,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="68" customFormat="1" spans="1:10">
-      <c r="A68" s="1" t="s">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>36</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B68" t="s">
         <v>11</v>
       </c>
       <c r="C68">
@@ -3357,11 +2765,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="69" customFormat="1" spans="1:10">
-      <c r="A69" s="1" t="s">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>36</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B69" t="s">
         <v>11</v>
       </c>
       <c r="C69">
@@ -3389,11 +2797,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="70" customFormat="1" spans="1:10">
-      <c r="A70" s="1" t="s">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>36</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B70" t="s">
         <v>11</v>
       </c>
       <c r="C70">
@@ -3421,11 +2829,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="71" customFormat="1" spans="1:10">
-      <c r="A71" s="1" t="s">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>37</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B71" t="s">
         <v>11</v>
       </c>
       <c r="C71">
@@ -3453,11 +2861,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="72" customFormat="1" spans="1:10">
-      <c r="A72" s="1" t="s">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>37</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="B72" t="s">
         <v>11</v>
       </c>
       <c r="C72">
@@ -3485,11 +2893,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="73" customFormat="1" spans="1:10">
-      <c r="A73" s="1" t="s">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>37</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="B73" t="s">
         <v>11</v>
       </c>
       <c r="C73">
@@ -3517,11 +2925,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="74" customFormat="1" spans="1:10">
-      <c r="A74" s="1" t="s">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>38</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="B74" t="s">
         <v>11</v>
       </c>
       <c r="C74">
@@ -3549,11 +2957,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="75" customFormat="1" spans="1:10">
-      <c r="A75" s="1" t="s">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>38</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B75" t="s">
         <v>11</v>
       </c>
       <c r="C75">
@@ -3581,11 +2989,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="76" customFormat="1" spans="1:10">
-      <c r="A76" s="1" t="s">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>38</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="B76" t="s">
         <v>11</v>
       </c>
       <c r="C76">
@@ -3613,11 +3021,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="77" customFormat="1" spans="1:10">
-      <c r="A77" s="1" t="s">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
         <v>39</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="B77" t="s">
         <v>11</v>
       </c>
       <c r="C77">
@@ -3645,11 +3053,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="78" customFormat="1" spans="1:10">
-      <c r="A78" s="1" t="s">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>39</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="B78" t="s">
         <v>11</v>
       </c>
       <c r="C78">
@@ -3677,11 +3085,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="79" customFormat="1" spans="1:10">
-      <c r="A79" s="1" t="s">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
         <v>39</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="B79" t="s">
         <v>11</v>
       </c>
       <c r="C79">
@@ -3709,11 +3117,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="80" customFormat="1" spans="1:10">
-      <c r="A80" s="1" t="s">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>40</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="B80" t="s">
         <v>11</v>
       </c>
       <c r="C80">
@@ -3741,11 +3149,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="81" customFormat="1" spans="1:10">
-      <c r="A81" s="1" t="s">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
         <v>40</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="B81" t="s">
         <v>11</v>
       </c>
       <c r="C81">
@@ -3773,11 +3181,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="82" customFormat="1" spans="1:10">
-      <c r="A82" s="1" t="s">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>40</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="B82" t="s">
         <v>11</v>
       </c>
       <c r="C82">
@@ -3805,11 +3213,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="83" customFormat="1" spans="1:10">
-      <c r="A83" s="1" t="s">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
         <v>41</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="B83" t="s">
         <v>11</v>
       </c>
       <c r="C83">
@@ -3837,11 +3245,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="84" customFormat="1" spans="1:10">
-      <c r="A84" s="1" t="s">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
         <v>41</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="B84" t="s">
         <v>11</v>
       </c>
       <c r="C84">
@@ -3869,11 +3277,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="85" customFormat="1" spans="1:10">
-      <c r="A85" s="1" t="s">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
         <v>41</v>
       </c>
-      <c r="B85" s="1" t="s">
+      <c r="B85" t="s">
         <v>11</v>
       </c>
       <c r="C85">
@@ -3901,11 +3309,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="86" customFormat="1" spans="1:10">
-      <c r="A86" s="1" t="s">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>42</v>
       </c>
-      <c r="B86" s="1" t="s">
+      <c r="B86" t="s">
         <v>11</v>
       </c>
       <c r="C86">
@@ -3933,11 +3341,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="87" customFormat="1" spans="1:10">
-      <c r="A87" s="1" t="s">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>42</v>
       </c>
-      <c r="B87" s="1" t="s">
+      <c r="B87" t="s">
         <v>11</v>
       </c>
       <c r="C87">
@@ -3965,11 +3373,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="88" customFormat="1" spans="1:10">
-      <c r="A88" s="1" t="s">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>42</v>
       </c>
-      <c r="B88" s="1" t="s">
+      <c r="B88" t="s">
         <v>11</v>
       </c>
       <c r="C88">
@@ -3997,11 +3405,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="89" customFormat="1" spans="1:10">
-      <c r="A89" s="1" t="s">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>43</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="B89" t="s">
         <v>11</v>
       </c>
       <c r="C89">
@@ -4029,11 +3437,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="90" customFormat="1" spans="1:10">
-      <c r="A90" s="1" t="s">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>43</v>
       </c>
-      <c r="B90" s="1" t="s">
+      <c r="B90" t="s">
         <v>11</v>
       </c>
       <c r="C90">
@@ -4061,11 +3469,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="91" customFormat="1" spans="1:10">
-      <c r="A91" s="1" t="s">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>43</v>
       </c>
-      <c r="B91" s="1" t="s">
+      <c r="B91" t="s">
         <v>11</v>
       </c>
       <c r="C91">
@@ -4093,11 +3501,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="92" customFormat="1" spans="1:10">
-      <c r="A92" s="1" t="s">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>44</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="B92" t="s">
         <v>11</v>
       </c>
       <c r="C92">
@@ -4125,11 +3533,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="93" customFormat="1" spans="1:10">
-      <c r="A93" s="1" t="s">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
         <v>44</v>
       </c>
-      <c r="B93" s="1" t="s">
+      <c r="B93" t="s">
         <v>11</v>
       </c>
       <c r="C93">
@@ -4157,11 +3565,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="94" customFormat="1" spans="1:10">
-      <c r="A94" s="1" t="s">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>44</v>
       </c>
-      <c r="B94" s="1" t="s">
+      <c r="B94" t="s">
         <v>11</v>
       </c>
       <c r="C94">
@@ -4189,11 +3597,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="95" customFormat="1" spans="1:10">
-      <c r="A95" s="1" t="s">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
         <v>45</v>
       </c>
-      <c r="B95" s="1" t="s">
+      <c r="B95" t="s">
         <v>11</v>
       </c>
       <c r="C95">
@@ -4209,23 +3617,23 @@
         <v>0</v>
       </c>
       <c r="G95">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H95">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I95">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J95" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="96" customFormat="1" spans="1:10">
-      <c r="A96" s="1" t="s">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>45</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="B96" t="s">
         <v>11</v>
       </c>
       <c r="C96">
@@ -4241,23 +3649,23 @@
         <v>0</v>
       </c>
       <c r="G96">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H96">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I96">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J96" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="97" customFormat="1" spans="1:10">
-      <c r="A97" s="1" t="s">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
         <v>45</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="B97" t="s">
         <v>11</v>
       </c>
       <c r="C97">
@@ -4273,23 +3681,23 @@
         <v>0</v>
       </c>
       <c r="G97">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H97">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I97">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J97" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="98" customFormat="1" spans="1:10">
-      <c r="A98" s="1" t="s">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
         <v>46</v>
       </c>
-      <c r="B98" s="1" t="s">
+      <c r="B98" t="s">
         <v>11</v>
       </c>
       <c r="C98">
@@ -4317,11 +3725,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="99" customFormat="1" spans="1:10">
-      <c r="A99" s="1" t="s">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
         <v>46</v>
       </c>
-      <c r="B99" s="1" t="s">
+      <c r="B99" t="s">
         <v>11</v>
       </c>
       <c r="C99">
@@ -4349,11 +3757,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="100" customFormat="1" spans="1:10">
-      <c r="A100" s="1" t="s">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
         <v>46</v>
       </c>
-      <c r="B100" s="1" t="s">
+      <c r="B100" t="s">
         <v>11</v>
       </c>
       <c r="C100">
@@ -4381,11 +3789,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="101" customFormat="1" spans="1:10">
-      <c r="A101" s="1" t="s">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
         <v>47</v>
       </c>
-      <c r="B101" s="1" t="s">
+      <c r="B101" t="s">
         <v>11</v>
       </c>
       <c r="C101">
@@ -4413,15 +3821,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="102" customFormat="1" spans="1:10">
-      <c r="A102" s="1" t="s">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
         <v>47</v>
       </c>
-      <c r="B102" s="1" t="s">
+      <c r="B102" t="s">
         <v>11</v>
       </c>
       <c r="C102">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D102">
         <v>0</v>
@@ -4445,11 +3853,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="103" customFormat="1" spans="1:10">
-      <c r="A103" s="1" t="s">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
         <v>47</v>
       </c>
-      <c r="B103" s="1" t="s">
+      <c r="B103" t="s">
         <v>11</v>
       </c>
       <c r="C103">
@@ -4477,11 +3885,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="104" customFormat="1" spans="1:10">
-      <c r="A104" s="1" t="s">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
         <v>48</v>
       </c>
-      <c r="B104" s="1" t="s">
+      <c r="B104" t="s">
         <v>11</v>
       </c>
       <c r="C104">
@@ -4509,11 +3917,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="105" customFormat="1" spans="1:10">
-      <c r="A105" s="1" t="s">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
         <v>48</v>
       </c>
-      <c r="B105" s="1" t="s">
+      <c r="B105" t="s">
         <v>11</v>
       </c>
       <c r="C105">
@@ -4523,7 +3931,7 @@
         <v>0</v>
       </c>
       <c r="E105">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F105">
         <v>0</v>
@@ -4541,11 +3949,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="106" customFormat="1" spans="1:10">
-      <c r="A106" s="1" t="s">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
         <v>48</v>
       </c>
-      <c r="B106" s="1" t="s">
+      <c r="B106" t="s">
         <v>11</v>
       </c>
       <c r="C106">
@@ -4573,11 +3981,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="107" customFormat="1" spans="1:10">
-      <c r="A107" s="1" t="s">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
         <v>49</v>
       </c>
-      <c r="B107" s="1" t="s">
+      <c r="B107" t="s">
         <v>11</v>
       </c>
       <c r="C107">
@@ -4605,11 +4013,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="108" customFormat="1" spans="1:10">
-      <c r="A108" s="1" t="s">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
         <v>49</v>
       </c>
-      <c r="B108" s="1" t="s">
+      <c r="B108" t="s">
         <v>11</v>
       </c>
       <c r="C108">
@@ -4637,11 +4045,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="109" customFormat="1" spans="1:10">
-      <c r="A109" s="1" t="s">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
         <v>49</v>
       </c>
-      <c r="B109" s="1" t="s">
+      <c r="B109" t="s">
         <v>11</v>
       </c>
       <c r="C109">
@@ -4669,11 +4077,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="110" customFormat="1" spans="1:10">
-      <c r="A110" s="1" t="s">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
         <v>50</v>
       </c>
-      <c r="B110" s="1" t="s">
+      <c r="B110" t="s">
         <v>11</v>
       </c>
       <c r="C110">
@@ -4689,23 +4097,23 @@
         <v>0</v>
       </c>
       <c r="G110">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H110">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I110">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J110" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="111" customFormat="1" spans="1:10">
-      <c r="A111" s="1" t="s">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
         <v>50</v>
       </c>
-      <c r="B111" s="1" t="s">
+      <c r="B111" t="s">
         <v>11</v>
       </c>
       <c r="C111">
@@ -4721,23 +4129,23 @@
         <v>0</v>
       </c>
       <c r="G111">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H111">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I111">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J111" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="112" customFormat="1" spans="1:10">
-      <c r="A112" s="1" t="s">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
         <v>50</v>
       </c>
-      <c r="B112" s="1" t="s">
+      <c r="B112" t="s">
         <v>11</v>
       </c>
       <c r="C112">
@@ -4753,23 +4161,23 @@
         <v>0</v>
       </c>
       <c r="G112">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H112">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I112">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J112" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="113" customFormat="1" spans="1:10">
-      <c r="A113" s="1" t="s">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
         <v>51</v>
       </c>
-      <c r="B113" s="1" t="s">
+      <c r="B113" t="s">
         <v>11</v>
       </c>
       <c r="C113">
@@ -4797,11 +4205,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="114" customFormat="1" spans="1:10">
-      <c r="A114" s="1" t="s">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
         <v>51</v>
       </c>
-      <c r="B114" s="1" t="s">
+      <c r="B114" t="s">
         <v>11</v>
       </c>
       <c r="C114">
@@ -4829,11 +4237,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="115" customFormat="1" spans="1:10">
-      <c r="A115" s="1" t="s">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
         <v>51</v>
       </c>
-      <c r="B115" s="1" t="s">
+      <c r="B115" t="s">
         <v>11</v>
       </c>
       <c r="C115">
@@ -4861,11 +4269,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="116" customFormat="1" spans="1:10">
-      <c r="A116" s="1" t="s">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
         <v>52</v>
       </c>
-      <c r="B116" s="1" t="s">
+      <c r="B116" t="s">
         <v>11</v>
       </c>
       <c r="C116">
@@ -4893,11 +4301,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="117" customFormat="1" spans="1:10">
-      <c r="A117" s="1" t="s">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
         <v>52</v>
       </c>
-      <c r="B117" s="1" t="s">
+      <c r="B117" t="s">
         <v>11</v>
       </c>
       <c r="C117">
@@ -4925,11 +4333,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="118" customFormat="1" spans="1:10">
-      <c r="A118" s="1" t="s">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
         <v>52</v>
       </c>
-      <c r="B118" s="1" t="s">
+      <c r="B118" t="s">
         <v>11</v>
       </c>
       <c r="C118">
@@ -4957,12 +4365,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="119" customFormat="1" spans="1:10">
-      <c r="A119" s="1" t="s">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>54</v>
+      </c>
+      <c r="B119" t="s">
         <v>53</v>
-      </c>
-      <c r="B119" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="C119">
         <v>0</v>
@@ -4989,12 +4397,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="120" customFormat="1" spans="1:10">
-      <c r="A120" s="1" t="s">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>54</v>
+      </c>
+      <c r="B120" t="s">
         <v>53</v>
-      </c>
-      <c r="B120" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="C120">
         <v>0</v>
@@ -5021,12 +4429,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="121" customFormat="1" spans="1:10">
-      <c r="A121" s="1" t="s">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>54</v>
+      </c>
+      <c r="B121" t="s">
         <v>53</v>
-      </c>
-      <c r="B121" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="C121">
         <v>0</v>
@@ -5053,12 +4461,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="122" customFormat="1" spans="1:10">
-      <c r="A122" s="1" t="s">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
         <v>55</v>
       </c>
-      <c r="B122" s="1" t="s">
-        <v>54</v>
+      <c r="B122" t="s">
+        <v>53</v>
       </c>
       <c r="C122">
         <v>0</v>
@@ -5085,12 +4493,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="123" customFormat="1" spans="1:10">
-      <c r="A123" s="1" t="s">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
         <v>55</v>
       </c>
-      <c r="B123" s="1" t="s">
-        <v>54</v>
+      <c r="B123" t="s">
+        <v>53</v>
       </c>
       <c r="C123">
         <v>0</v>
@@ -5117,12 +4525,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="124" customFormat="1" spans="1:10">
-      <c r="A124" s="1" t="s">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
         <v>55</v>
       </c>
-      <c r="B124" s="1" t="s">
-        <v>54</v>
+      <c r="B124" t="s">
+        <v>53</v>
       </c>
       <c r="C124">
         <v>0</v>
@@ -5149,12 +4557,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="125" customFormat="1" spans="1:10">
-      <c r="A125" s="1" t="s">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
         <v>56</v>
       </c>
-      <c r="B125" s="1" t="s">
-        <v>54</v>
+      <c r="B125" t="s">
+        <v>53</v>
       </c>
       <c r="C125">
         <v>0</v>
@@ -5181,12 +4589,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="126" customFormat="1" spans="1:10">
-      <c r="A126" s="1" t="s">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
         <v>56</v>
       </c>
-      <c r="B126" s="1" t="s">
-        <v>54</v>
+      <c r="B126" t="s">
+        <v>53</v>
       </c>
       <c r="C126">
         <v>0</v>
@@ -5213,12 +4621,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="127" customFormat="1" spans="1:10">
-      <c r="A127" s="1" t="s">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
         <v>56</v>
       </c>
-      <c r="B127" s="1" t="s">
-        <v>54</v>
+      <c r="B127" t="s">
+        <v>53</v>
       </c>
       <c r="C127">
         <v>1</v>
@@ -5245,12 +4653,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="128" customFormat="1" spans="1:10">
-      <c r="A128" s="1" t="s">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
         <v>57</v>
       </c>
-      <c r="B128" s="1" t="s">
-        <v>54</v>
+      <c r="B128" t="s">
+        <v>53</v>
       </c>
       <c r="C128">
         <v>1</v>
@@ -5277,12 +4685,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="129" customFormat="1" spans="1:10">
-      <c r="A129" s="1" t="s">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
         <v>57</v>
       </c>
-      <c r="B129" s="1" t="s">
-        <v>54</v>
+      <c r="B129" t="s">
+        <v>53</v>
       </c>
       <c r="C129">
         <v>1</v>
@@ -5309,12 +4717,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="130" customFormat="1" spans="1:10">
-      <c r="A130" s="1" t="s">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
         <v>57</v>
       </c>
-      <c r="B130" s="1" t="s">
-        <v>54</v>
+      <c r="B130" t="s">
+        <v>53</v>
       </c>
       <c r="C130">
         <v>1</v>
@@ -5341,12 +4749,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="131" customFormat="1" spans="1:10">
-      <c r="A131" s="1" t="s">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
         <v>58</v>
       </c>
-      <c r="B131" s="1" t="s">
-        <v>54</v>
+      <c r="B131" t="s">
+        <v>53</v>
       </c>
       <c r="C131">
         <v>0</v>
@@ -5373,12 +4781,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="132" customFormat="1" spans="1:10">
-      <c r="A132" s="1" t="s">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
         <v>58</v>
       </c>
-      <c r="B132" s="1" t="s">
-        <v>54</v>
+      <c r="B132" t="s">
+        <v>53</v>
       </c>
       <c r="C132">
         <v>0</v>
@@ -5405,12 +4813,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="133" customFormat="1" spans="1:10">
-      <c r="A133" s="1" t="s">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
         <v>58</v>
       </c>
-      <c r="B133" s="1" t="s">
-        <v>54</v>
+      <c r="B133" t="s">
+        <v>53</v>
       </c>
       <c r="C133">
         <v>0</v>
@@ -5437,12 +4845,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="134" customFormat="1" spans="1:10">
-      <c r="A134" s="1" t="s">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
         <v>59</v>
       </c>
-      <c r="B134" s="1" t="s">
-        <v>54</v>
+      <c r="B134" t="s">
+        <v>53</v>
       </c>
       <c r="C134">
         <v>0</v>
@@ -5469,12 +4877,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="135" customFormat="1" spans="1:10">
-      <c r="A135" s="1" t="s">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
         <v>59</v>
       </c>
-      <c r="B135" s="1" t="s">
-        <v>54</v>
+      <c r="B135" t="s">
+        <v>53</v>
       </c>
       <c r="C135">
         <v>0</v>
@@ -5501,12 +4909,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="136" customFormat="1" spans="1:10">
-      <c r="A136" s="1" t="s">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
         <v>59</v>
       </c>
-      <c r="B136" s="1" t="s">
-        <v>54</v>
+      <c r="B136" t="s">
+        <v>53</v>
       </c>
       <c r="C136">
         <v>0</v>
@@ -5533,12 +4941,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="137" customFormat="1" spans="1:10">
-      <c r="A137" s="1" t="s">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
         <v>60</v>
       </c>
-      <c r="B137" s="1" t="s">
-        <v>54</v>
+      <c r="B137" t="s">
+        <v>53</v>
       </c>
       <c r="C137">
         <v>0</v>
@@ -5565,12 +4973,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="138" customFormat="1" spans="1:10">
-      <c r="A138" s="1" t="s">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
         <v>60</v>
       </c>
-      <c r="B138" s="1" t="s">
-        <v>54</v>
+      <c r="B138" t="s">
+        <v>53</v>
       </c>
       <c r="C138">
         <v>0</v>
@@ -5597,12 +5005,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="139" customFormat="1" spans="1:10">
-      <c r="A139" s="1" t="s">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
         <v>60</v>
       </c>
-      <c r="B139" s="1" t="s">
-        <v>54</v>
+      <c r="B139" t="s">
+        <v>53</v>
       </c>
       <c r="C139">
         <v>0</v>
@@ -5629,12 +5037,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="140" customFormat="1" spans="1:10">
-      <c r="A140" s="1" t="s">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
         <v>61</v>
       </c>
-      <c r="B140" s="1" t="s">
-        <v>54</v>
+      <c r="B140" t="s">
+        <v>53</v>
       </c>
       <c r="C140">
         <v>0</v>
@@ -5649,24 +5057,24 @@
         <v>0</v>
       </c>
       <c r="G140">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H140">
         <v>0</v>
       </c>
       <c r="I140">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J140" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="141" customFormat="1" spans="1:10">
-      <c r="A141" s="1" t="s">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
         <v>61</v>
       </c>
-      <c r="B141" s="1" t="s">
-        <v>54</v>
+      <c r="B141" t="s">
+        <v>53</v>
       </c>
       <c r="C141">
         <v>0</v>
@@ -5675,13 +5083,13 @@
         <v>1</v>
       </c>
       <c r="E141">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F141">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G141">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H141">
         <v>0</v>
@@ -5693,12 +5101,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="142" customFormat="1" spans="1:10">
-      <c r="A142" s="1" t="s">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
         <v>61</v>
       </c>
-      <c r="B142" s="1" t="s">
-        <v>54</v>
+      <c r="B142" t="s">
+        <v>53</v>
       </c>
       <c r="C142">
         <v>0</v>
@@ -5713,24 +5121,24 @@
         <v>0</v>
       </c>
       <c r="G142">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H142">
         <v>0</v>
       </c>
       <c r="I142">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J142" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="143" customFormat="1" spans="1:10">
-      <c r="A143" s="1" t="s">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
         <v>62</v>
       </c>
-      <c r="B143" s="1" t="s">
-        <v>54</v>
+      <c r="B143" t="s">
+        <v>53</v>
       </c>
       <c r="C143">
         <v>0</v>
@@ -5757,12 +5165,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="144" customFormat="1" spans="1:10">
-      <c r="A144" s="1" t="s">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
         <v>62</v>
       </c>
-      <c r="B144" s="1" t="s">
-        <v>54</v>
+      <c r="B144" t="s">
+        <v>53</v>
       </c>
       <c r="C144">
         <v>0</v>
@@ -5789,12 +5197,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="145" customFormat="1" spans="1:10">
-      <c r="A145" s="1" t="s">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
         <v>62</v>
       </c>
-      <c r="B145" s="1" t="s">
-        <v>54</v>
+      <c r="B145" t="s">
+        <v>53</v>
       </c>
       <c r="C145">
         <v>0</v>
@@ -5821,12 +5229,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="146" customFormat="1" spans="1:10">
-      <c r="A146" s="1" t="s">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
         <v>63</v>
       </c>
-      <c r="B146" s="1" t="s">
-        <v>54</v>
+      <c r="B146" t="s">
+        <v>53</v>
       </c>
       <c r="C146">
         <v>0</v>
@@ -5853,12 +5261,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="147" customFormat="1" spans="1:10">
-      <c r="A147" s="1" t="s">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
         <v>63</v>
       </c>
-      <c r="B147" s="1" t="s">
-        <v>54</v>
+      <c r="B147" t="s">
+        <v>53</v>
       </c>
       <c r="C147">
         <v>0</v>
@@ -5885,12 +5293,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="148" customFormat="1" spans="1:10">
-      <c r="A148" s="1" t="s">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
         <v>63</v>
       </c>
-      <c r="B148" s="1" t="s">
-        <v>54</v>
+      <c r="B148" t="s">
+        <v>53</v>
       </c>
       <c r="C148">
         <v>0</v>
@@ -5917,12 +5325,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="149" customFormat="1" spans="1:10">
-      <c r="A149" s="1" t="s">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
         <v>64</v>
       </c>
-      <c r="B149" s="1" t="s">
-        <v>54</v>
+      <c r="B149" t="s">
+        <v>53</v>
       </c>
       <c r="C149">
         <v>0</v>
@@ -5937,24 +5345,24 @@
         <v>0</v>
       </c>
       <c r="G149">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H149">
         <v>0</v>
       </c>
       <c r="I149">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J149" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="150" customFormat="1" spans="1:10">
-      <c r="A150" s="1" t="s">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
         <v>64</v>
       </c>
-      <c r="B150" s="1" t="s">
-        <v>54</v>
+      <c r="B150" t="s">
+        <v>53</v>
       </c>
       <c r="C150">
         <v>0</v>
@@ -5963,13 +5371,13 @@
         <v>1</v>
       </c>
       <c r="E150">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F150">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G150">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H150">
         <v>0</v>
@@ -5981,12 +5389,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="151" customFormat="1" spans="1:10">
-      <c r="A151" s="1" t="s">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
         <v>64</v>
       </c>
-      <c r="B151" s="1" t="s">
-        <v>54</v>
+      <c r="B151" t="s">
+        <v>53</v>
       </c>
       <c r="C151">
         <v>0</v>
@@ -6001,24 +5409,24 @@
         <v>0</v>
       </c>
       <c r="G151">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H151">
         <v>0</v>
       </c>
       <c r="I151">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J151" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="152" customFormat="1" spans="1:10">
-      <c r="A152" s="1" t="s">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
         <v>65</v>
       </c>
-      <c r="B152" s="1" t="s">
-        <v>54</v>
+      <c r="B152" t="s">
+        <v>53</v>
       </c>
       <c r="C152">
         <v>0</v>
@@ -6045,12 +5453,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="153" customFormat="1" spans="1:10">
-      <c r="A153" s="1" t="s">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
         <v>65</v>
       </c>
-      <c r="B153" s="1" t="s">
-        <v>54</v>
+      <c r="B153" t="s">
+        <v>53</v>
       </c>
       <c r="C153">
         <v>0</v>
@@ -6077,12 +5485,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="154" customFormat="1" spans="1:10">
-      <c r="A154" s="1" t="s">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
         <v>65</v>
       </c>
-      <c r="B154" s="1" t="s">
-        <v>54</v>
+      <c r="B154" t="s">
+        <v>53</v>
       </c>
       <c r="C154">
         <v>0</v>
@@ -6109,46 +5517,232 @@
         <v>14</v>
       </c>
     </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A155" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B155" t="s">
+        <v>53</v>
+      </c>
+      <c r="C155">
+        <v>1</v>
+      </c>
+      <c r="D155">
+        <v>0</v>
+      </c>
+      <c r="E155">
+        <v>1</v>
+      </c>
+      <c r="F155">
+        <v>0</v>
+      </c>
+      <c r="G155">
+        <v>1</v>
+      </c>
+      <c r="H155">
+        <v>1</v>
+      </c>
+      <c r="I155">
+        <v>1</v>
+      </c>
+      <c r="J155" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A156" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B156" t="s">
+        <v>53</v>
+      </c>
+      <c r="C156">
+        <v>0</v>
+      </c>
+      <c r="D156">
+        <v>1</v>
+      </c>
+      <c r="E156">
+        <v>0</v>
+      </c>
+      <c r="F156">
+        <v>1</v>
+      </c>
+      <c r="G156">
+        <v>1</v>
+      </c>
+      <c r="H156">
+        <v>0</v>
+      </c>
+      <c r="I156">
+        <v>0</v>
+      </c>
+      <c r="J156" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A157" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B157" t="s">
+        <v>53</v>
+      </c>
+      <c r="C157">
+        <v>0</v>
+      </c>
+      <c r="D157">
+        <v>1</v>
+      </c>
+      <c r="E157">
+        <v>1</v>
+      </c>
+      <c r="F157">
+        <v>0</v>
+      </c>
+      <c r="G157">
+        <v>1</v>
+      </c>
+      <c r="H157">
+        <v>0</v>
+      </c>
+      <c r="I157">
+        <v>1</v>
+      </c>
+      <c r="J157" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A158" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B158" t="s">
+        <v>53</v>
+      </c>
+      <c r="C158">
+        <v>0</v>
+      </c>
+      <c r="D158">
+        <v>1</v>
+      </c>
+      <c r="E158">
+        <v>1</v>
+      </c>
+      <c r="F158">
+        <v>1</v>
+      </c>
+      <c r="G158">
+        <v>0</v>
+      </c>
+      <c r="H158">
+        <v>0</v>
+      </c>
+      <c r="I158">
+        <v>0</v>
+      </c>
+      <c r="J158" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A159" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B159" t="s">
+        <v>53</v>
+      </c>
+      <c r="C159">
+        <v>0</v>
+      </c>
+      <c r="D159">
+        <v>1</v>
+      </c>
+      <c r="E159">
+        <v>1</v>
+      </c>
+      <c r="F159">
+        <v>0</v>
+      </c>
+      <c r="G159">
+        <v>0</v>
+      </c>
+      <c r="H159">
+        <v>0</v>
+      </c>
+      <c r="I159">
+        <v>0</v>
+      </c>
+      <c r="J159" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A160" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B160" t="s">
+        <v>53</v>
+      </c>
+      <c r="C160">
+        <v>0</v>
+      </c>
+      <c r="D160">
+        <v>1</v>
+      </c>
+      <c r="E160">
+        <v>1</v>
+      </c>
+      <c r="F160">
+        <v>0</v>
+      </c>
+      <c r="G160">
+        <v>0</v>
+      </c>
+      <c r="H160">
+        <v>0</v>
+      </c>
+      <c r="I160">
+        <v>0</v>
+      </c>
+      <c r="J160" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A1:H151">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:H151">
     <sortCondition ref="A127"/>
   </sortState>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <sheetData/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <sheetData/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>